<commit_message>
# excel file updated
</commit_message>
<xml_diff>
--- a/py_mail_test.xlsx
+++ b/py_mail_test.xlsx
@@ -34,10 +34,10 @@
       <rPr>
         <u val="single"/>
         <sz val="10"/>
-        <color indexed="8"/>
+        <color indexed="15"/>
         <rFont val="ヒラギノ角ゴ ProN W3"/>
       </rPr>
-      <t>rusami@outlook.jp</t>
+      <t>rusami-2020@outlook.jp</t>
     </r>
   </si>
 </sst>
@@ -48,7 +48,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -60,6 +60,12 @@
       <name val="ヒラギノ角ゴ ProN W3"/>
     </font>
     <font>
+      <sz val="15"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="1"/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="ヒラギノ角ゴ ProN W6"/>
@@ -70,8 +76,14 @@
       <color indexed="8"/>
       <name val="ヒラギノ角ゴ ProN W3"/>
     </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color indexed="15"/>
+      <name val="ヒラギノ角ゴ ProN W3"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -90,8 +102,14 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="14"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -103,6 +121,28 @@
       <left style="thin">
         <color indexed="10"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="10"/>
       </right>
@@ -116,7 +156,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
         <color indexed="11"/>
@@ -125,7 +165,7 @@
         <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -134,43 +174,43 @@
         <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
         <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -179,28 +219,43 @@
         <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -210,38 +265,44 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -261,10 +322,13 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="ff0000ff"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -281,10 +345,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="5E5E5E"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="D5D5D5"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="00A2FF"/>
@@ -461,11 +525,14 @@
     <a:spDef>
       <a:spPr>
         <a:solidFill>
-          <a:srgbClr val="000000"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -474,27 +541,27 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="584200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
@@ -749,12 +816,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="000000"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1045,7 +1112,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1323,16 +1390,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:G23"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.6" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="9.125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="27.5703" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.21094" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.6016" style="1" customWidth="1"/>
     <col min="3" max="7" width="19.6016" style="1" customWidth="1"/>
     <col min="8" max="16384" width="19.6016" style="1" customWidth="1"/>
   </cols>
@@ -1341,216 +1406,216 @@
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="4"/>
     </row>
     <row r="2" ht="18.5" customHeight="1">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
     </row>
     <row r="3" ht="18.5" customHeight="1">
-      <c r="A3" s="4"/>
-      <c r="B3" t="s" s="5">
+      <c r="A3" s="6"/>
+      <c r="B3" t="s" s="7">
         <v>1</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
     </row>
     <row r="4" ht="18.3" customHeight="1">
-      <c r="A4" s="7"/>
-      <c r="B4" t="s" s="8">
+      <c r="A4" s="9"/>
+      <c r="B4" t="s" s="10">
         <v>2</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
     </row>
     <row r="5" ht="18.55" customHeight="1">
-      <c r="A5" s="7"/>
-      <c r="B5" t="s" s="8">
+      <c r="A5" s="9"/>
+      <c r="B5" t="s" s="10">
         <v>3</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
     </row>
     <row r="6" ht="18.3" customHeight="1">
-      <c r="A6" s="7"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
+      <c r="A6" s="9"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
     </row>
     <row r="7" ht="18.3" customHeight="1">
-      <c r="A7" s="7"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
     </row>
     <row r="8" ht="18.3" customHeight="1">
-      <c r="A8" s="7"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
     </row>
     <row r="9" ht="18.3" customHeight="1">
-      <c r="A9" s="7"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
     </row>
     <row r="10" ht="18.3" customHeight="1">
-      <c r="A10" s="7"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
     </row>
     <row r="11" ht="18.3" customHeight="1">
-      <c r="A11" s="7"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
+      <c r="A11" s="9"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
     </row>
     <row r="12" ht="18.3" customHeight="1">
-      <c r="A12" s="7"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
+      <c r="A12" s="9"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
     </row>
     <row r="13" ht="18.3" customHeight="1">
-      <c r="A13" s="7"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
+      <c r="A13" s="9"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
     </row>
     <row r="14" ht="18.3" customHeight="1">
-      <c r="A14" s="7"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
+      <c r="A14" s="9"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
     </row>
     <row r="15" ht="18.3" customHeight="1">
-      <c r="A15" s="7"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
     </row>
     <row r="16" ht="18.3" customHeight="1">
-      <c r="A16" s="7"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
     </row>
     <row r="17" ht="18.3" customHeight="1">
-      <c r="A17" s="7"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
+      <c r="A17" s="9"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
     </row>
     <row r="18" ht="18.3" customHeight="1">
-      <c r="A18" s="7"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
+      <c r="A18" s="9"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
     </row>
     <row r="19" ht="18.3" customHeight="1">
-      <c r="A19" s="7"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
+      <c r="A19" s="9"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
     </row>
     <row r="20" ht="18.3" customHeight="1">
-      <c r="A20" s="7"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
+      <c r="A20" s="9"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
     </row>
     <row r="21" ht="18.3" customHeight="1">
-      <c r="A21" s="7"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
+      <c r="A21" s="9"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
     </row>
     <row r="22" ht="18.3" customHeight="1">
-      <c r="A22" s="7"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
+      <c r="A22" s="9"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
     </row>
     <row r="23" ht="18.3" customHeight="1">
-      <c r="A23" s="7"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
+      <c r="A23" s="9"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1558,7 +1623,7 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" location="" tooltip="" display="rusami.usual@icloud.com"/>
-    <hyperlink ref="B5" r:id="rId2" location="" tooltip="" display="rusami@outlook.jp"/>
+    <hyperlink ref="B5" r:id="rId2" location="" tooltip="" display="rusami-2020@outlook.jp"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>